<commit_message>
cierre 10 Ene 2022
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE  HERRADURA  DICIEMBRE   2021.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL  ARCHIVO  2 0 2 1/CENTRAL # 12  DICIEMBRE   2021/BALANCE  HERRADURA  DICIEMBRE   2021.xlsx
@@ -325,7 +325,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="334">
   <si>
     <t>COMPRAS</t>
   </si>
@@ -1299,10 +1299,34 @@
     <t>COMPRA VARIOS PRODUCTOS</t>
   </si>
   <si>
-    <t>NOMINA</t>
-  </si>
-  <si>
     <t>CREMA-TOTOPOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPRAS CENTRAL </t>
+  </si>
+  <si>
+    <t>NOMINA # 52</t>
+  </si>
+  <si>
+    <t>nomina 51 Aguinaldos</t>
+  </si>
+  <si>
+    <t>NOMINA 50</t>
+  </si>
+  <si>
+    <t>FESTIVO</t>
+  </si>
+  <si>
+    <t>PAVO NATURAL</t>
+  </si>
+  <si>
+    <t>BONOS DE ASISTENCIA</t>
+  </si>
+  <si>
+    <t>NOMINA # 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LONGANIZA-CENTRAL VARIOS  </t>
   </si>
 </sst>
 </file>
@@ -1681,7 +1705,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1733,6 +1757,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF33CCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2507,7 +2543,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="287">
+  <cellXfs count="308">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
@@ -2977,6 +3013,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="20" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="10" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="10" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="2" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="10" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="17" fillId="10" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="10" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3103,6 +3151,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="44" fontId="17" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="2" fillId="11" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="12" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="11" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="2" fillId="11" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="11" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="20" fillId="11" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="17" fillId="11" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="11" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -5550,23 +5611,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="270"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="280"/>
+      <c r="C1" s="289" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
+      <c r="I1" s="290"/>
+      <c r="J1" s="290"/>
+      <c r="K1" s="290"/>
+      <c r="L1" s="290"/>
+      <c r="M1" s="290"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="271"/>
+      <c r="B2" s="281"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -5576,17 +5637,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="273"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="274" t="s">
+      <c r="H3" s="284" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="274"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -5602,14 +5663,14 @@
       <c r="D4" s="16">
         <v>44410</v>
       </c>
-      <c r="E4" s="275" t="s">
+      <c r="E4" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="276"/>
-      <c r="H4" s="277" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="278"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -5619,10 +5680,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="264" t="s">
+      <c r="P4" s="274" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="265"/>
+      <c r="Q4" s="275"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -7117,11 +7178,11 @@
       <c r="L39" s="69">
         <v>454.62</v>
       </c>
-      <c r="M39" s="266">
+      <c r="M39" s="276">
         <f>SUM(M5:M38)</f>
         <v>1393675.5</v>
       </c>
-      <c r="N39" s="268">
+      <c r="N39" s="278">
         <f>SUM(N5:N38)</f>
         <v>28399.97</v>
       </c>
@@ -7153,8 +7214,8 @@
       <c r="L40" s="69">
         <v>1195.67</v>
       </c>
-      <c r="M40" s="267"/>
-      <c r="N40" s="269"/>
+      <c r="M40" s="277"/>
+      <c r="N40" s="279"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -7387,29 +7448,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="254" t="s">
+      <c r="H52" s="264" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="255"/>
+      <c r="I52" s="265"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="256">
+      <c r="K52" s="266">
         <f>I50+L50</f>
         <v>80916.84</v>
       </c>
-      <c r="L52" s="257"/>
-      <c r="M52" s="245">
+      <c r="L52" s="267"/>
+      <c r="M52" s="255">
         <f>N39+M39</f>
         <v>1422075.47</v>
       </c>
-      <c r="N52" s="246"/>
+      <c r="N52" s="256"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="258" t="s">
+      <c r="D53" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="258"/>
+      <c r="E53" s="268"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1396181.44</v>
@@ -7420,22 +7481,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="259" t="s">
+      <c r="D54" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="259"/>
+      <c r="E54" s="269"/>
       <c r="F54" s="102">
         <v>-1523111</v>
       </c>
-      <c r="I54" s="260" t="s">
+      <c r="I54" s="270" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="261"/>
-      <c r="K54" s="262">
+      <c r="J54" s="271"/>
+      <c r="K54" s="272">
         <f>F56+F57+F58</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L54" s="263"/>
+      <c r="L54" s="273"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -7466,10 +7527,10 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="247">
-        <v>0</v>
-      </c>
-      <c r="L56" s="248"/>
+      <c r="K56" s="257">
+        <v>0</v>
+      </c>
+      <c r="L56" s="258"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -7486,22 +7547,22 @@
       <c r="C58" s="120">
         <v>44444</v>
       </c>
-      <c r="D58" s="249" t="s">
+      <c r="D58" s="259" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="250"/>
+      <c r="E58" s="260"/>
       <c r="F58" s="121">
         <v>136234.76999999999</v>
       </c>
-      <c r="I58" s="251" t="s">
+      <c r="I58" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="252"/>
-      <c r="K58" s="253">
+      <c r="J58" s="262"/>
+      <c r="K58" s="263">
         <f>K54+K56</f>
         <v>9305.2099999999336</v>
       </c>
-      <c r="L58" s="253"/>
+      <c r="L58" s="263"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -9044,12 +9105,12 @@
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="163"/>
-      <c r="B45" s="284" t="s">
+      <c r="B45" s="294" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="285"/>
-      <c r="D45" s="285"/>
-      <c r="E45" s="286"/>
+      <c r="C45" s="295"/>
+      <c r="D45" s="295"/>
+      <c r="E45" s="296"/>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -9276,7 +9337,7 @@
       <c r="C3" s="35">
         <v>3015.96</v>
       </c>
-      <c r="D3" s="281" t="s">
+      <c r="D3" s="291" t="s">
         <v>49</v>
       </c>
       <c r="E3" s="9"/>
@@ -9295,7 +9356,7 @@
       <c r="C4" s="35">
         <v>10281</v>
       </c>
-      <c r="D4" s="282"/>
+      <c r="D4" s="292"/>
       <c r="E4" s="180"/>
       <c r="F4" s="145">
         <f>F3+C4-E4</f>
@@ -9313,7 +9374,7 @@
       <c r="C5" s="35">
         <v>12746.2</v>
       </c>
-      <c r="D5" s="282"/>
+      <c r="D5" s="292"/>
       <c r="E5" s="180"/>
       <c r="F5" s="145">
         <f t="shared" ref="F5:F68" si="0">F4+C5-E5</f>
@@ -9330,7 +9391,7 @@
       <c r="C6" s="35">
         <v>28974.78</v>
       </c>
-      <c r="D6" s="282"/>
+      <c r="D6" s="292"/>
       <c r="E6" s="180"/>
       <c r="F6" s="145">
         <f t="shared" si="0"/>
@@ -9347,7 +9408,7 @@
       <c r="C7" s="35">
         <v>44758.6</v>
       </c>
-      <c r="D7" s="282"/>
+      <c r="D7" s="292"/>
       <c r="E7" s="180"/>
       <c r="F7" s="145">
         <f t="shared" si="0"/>
@@ -9364,7 +9425,7 @@
       <c r="C8" s="35">
         <v>12841.78</v>
       </c>
-      <c r="D8" s="282"/>
+      <c r="D8" s="292"/>
       <c r="E8" s="180"/>
       <c r="F8" s="145">
         <f t="shared" si="0"/>
@@ -9381,7 +9442,7 @@
       <c r="C9" s="35">
         <v>3898.05</v>
       </c>
-      <c r="D9" s="282"/>
+      <c r="D9" s="292"/>
       <c r="E9" s="180"/>
       <c r="F9" s="145">
         <f t="shared" si="0"/>
@@ -9398,7 +9459,7 @@
       <c r="C10" s="35">
         <v>1429</v>
       </c>
-      <c r="D10" s="283"/>
+      <c r="D10" s="293"/>
       <c r="E10" s="180"/>
       <c r="F10" s="145">
         <f t="shared" si="0"/>
@@ -10918,23 +10979,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="270"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="280"/>
+      <c r="C1" s="289" t="s">
         <v>112</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
+      <c r="I1" s="290"/>
+      <c r="J1" s="290"/>
+      <c r="K1" s="290"/>
+      <c r="L1" s="290"/>
+      <c r="M1" s="290"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="271"/>
+      <c r="B2" s="281"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -10944,17 +11005,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="273"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="274" t="s">
+      <c r="H3" s="284" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="274"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -10970,14 +11031,14 @@
       <c r="D4" s="16">
         <v>44444</v>
       </c>
-      <c r="E4" s="275" t="s">
+      <c r="E4" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="276"/>
-      <c r="H4" s="277" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="278"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -10987,10 +11048,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="264" t="s">
+      <c r="P4" s="274" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="265"/>
+      <c r="Q4" s="275"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -12480,11 +12541,11 @@
       <c r="J39" s="67"/>
       <c r="K39" s="82"/>
       <c r="L39" s="69"/>
-      <c r="M39" s="266">
+      <c r="M39" s="276">
         <f>SUM(M5:M38)</f>
         <v>1464441</v>
       </c>
-      <c r="N39" s="268">
+      <c r="N39" s="278">
         <f>SUM(N5:N38)</f>
         <v>53494</v>
       </c>
@@ -12510,8 +12571,8 @@
       <c r="J40" s="67"/>
       <c r="K40" s="71"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="267"/>
-      <c r="N40" s="269"/>
+      <c r="M40" s="277"/>
+      <c r="N40" s="279"/>
       <c r="P40" s="83"/>
       <c r="Q40" s="9"/>
     </row>
@@ -12726,29 +12787,29 @@
       <c r="A52" s="104"/>
       <c r="B52" s="105"/>
       <c r="C52" s="3"/>
-      <c r="H52" s="254" t="s">
+      <c r="H52" s="264" t="s">
         <v>8</v>
       </c>
-      <c r="I52" s="255"/>
+      <c r="I52" s="265"/>
       <c r="J52" s="106"/>
-      <c r="K52" s="256">
+      <c r="K52" s="266">
         <f>I50+L50</f>
         <v>69642.26999999999</v>
       </c>
-      <c r="L52" s="257"/>
-      <c r="M52" s="245">
+      <c r="L52" s="267"/>
+      <c r="M52" s="255">
         <f>N39+M39</f>
         <v>1517935</v>
       </c>
-      <c r="N52" s="246"/>
+      <c r="N52" s="256"/>
       <c r="P52" s="83"/>
       <c r="Q52" s="9"/>
     </row>
     <row r="53" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D53" s="258" t="s">
+      <c r="D53" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="258"/>
+      <c r="E53" s="268"/>
       <c r="F53" s="107">
         <f>F50-K52-C50</f>
         <v>1505921.23</v>
@@ -12759,22 +12820,22 @@
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D54" s="259" t="s">
+      <c r="D54" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="259"/>
+      <c r="E54" s="269"/>
       <c r="F54" s="102">
         <v>-1424333.95</v>
       </c>
-      <c r="I54" s="260" t="s">
+      <c r="I54" s="270" t="s">
         <v>11</v>
       </c>
-      <c r="J54" s="261"/>
-      <c r="K54" s="262">
+      <c r="J54" s="271"/>
+      <c r="K54" s="272">
         <f>F56+F57+F58</f>
         <v>222140.17000000004</v>
       </c>
-      <c r="L54" s="263"/>
+      <c r="L54" s="273"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="9"/>
     </row>
@@ -12805,11 +12866,11 @@
         <v>13</v>
       </c>
       <c r="J56" s="117"/>
-      <c r="K56" s="247">
+      <c r="K56" s="257">
         <f>-C4</f>
         <v>-136234.76999999999</v>
       </c>
-      <c r="L56" s="248"/>
+      <c r="L56" s="258"/>
     </row>
     <row r="57" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="118" t="s">
@@ -12826,22 +12887,22 @@
       <c r="C58" s="120">
         <v>44472</v>
       </c>
-      <c r="D58" s="249" t="s">
+      <c r="D58" s="259" t="s">
         <v>16</v>
       </c>
-      <c r="E58" s="250"/>
+      <c r="E58" s="260"/>
       <c r="F58" s="121">
         <v>134848.89000000001</v>
       </c>
-      <c r="I58" s="251" t="s">
+      <c r="I58" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="J58" s="252"/>
-      <c r="K58" s="253">
+      <c r="J58" s="262"/>
+      <c r="K58" s="263">
         <f>K54+K56</f>
         <v>85905.400000000052</v>
       </c>
-      <c r="L58" s="253"/>
+      <c r="L58" s="263"/>
     </row>
     <row r="59" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C59" s="122"/>
@@ -14628,23 +14689,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="270"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="280"/>
+      <c r="C1" s="289" t="s">
         <v>185</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
+      <c r="I1" s="290"/>
+      <c r="J1" s="290"/>
+      <c r="K1" s="290"/>
+      <c r="L1" s="290"/>
+      <c r="M1" s="290"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="271"/>
+      <c r="B2" s="281"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -14654,17 +14715,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="273"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="274" t="s">
+      <c r="H3" s="284" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="274"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -14680,14 +14741,14 @@
       <c r="D4" s="16">
         <v>44472</v>
       </c>
-      <c r="E4" s="275" t="s">
+      <c r="E4" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="276"/>
-      <c r="H4" s="277" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="278"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -14697,10 +14758,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="264" t="s">
+      <c r="P4" s="274" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="265"/>
+      <c r="Q4" s="275"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -16275,11 +16336,11 @@
       <c r="L40" s="69">
         <v>1195.68</v>
       </c>
-      <c r="M40" s="266">
+      <c r="M40" s="276">
         <f>SUM(M5:M39)</f>
         <v>1982944.5</v>
       </c>
-      <c r="N40" s="268">
+      <c r="N40" s="278">
         <f>SUM(N5:N39)</f>
         <v>62048</v>
       </c>
@@ -16311,8 +16372,8 @@
       <c r="L41" s="69">
         <v>942.84</v>
       </c>
-      <c r="M41" s="267"/>
-      <c r="N41" s="269"/>
+      <c r="M41" s="277"/>
+      <c r="N41" s="279"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -16545,29 +16606,29 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="254" t="s">
+      <c r="H53" s="264" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="255"/>
+      <c r="I53" s="265"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="256">
+      <c r="K53" s="266">
         <f>I51+L51</f>
         <v>104139.16999999998</v>
       </c>
-      <c r="L53" s="257"/>
-      <c r="M53" s="245">
+      <c r="L53" s="267"/>
+      <c r="M53" s="255">
         <f>N40+M40</f>
         <v>2044992.5</v>
       </c>
-      <c r="N53" s="246"/>
+      <c r="N53" s="256"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="258" t="s">
+      <c r="D54" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="258"/>
+      <c r="E54" s="268"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
         <v>2004605.33</v>
@@ -16578,22 +16639,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="259" t="s">
+      <c r="D55" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="259"/>
+      <c r="E55" s="269"/>
       <c r="F55" s="102">
         <v>-2026393.17</v>
       </c>
-      <c r="I55" s="260" t="s">
+      <c r="I55" s="270" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="261"/>
-      <c r="K55" s="262">
+      <c r="J55" s="271"/>
+      <c r="K55" s="272">
         <f>F57+F58+F59</f>
         <v>178711.56000000014</v>
       </c>
-      <c r="L55" s="263"/>
+      <c r="L55" s="273"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -16624,11 +16685,11 @@
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="247">
+      <c r="K57" s="257">
         <f>-C4</f>
         <v>-134848.89000000001</v>
       </c>
-      <c r="L57" s="248"/>
+      <c r="L57" s="258"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -16645,22 +16706,22 @@
       <c r="C59" s="120">
         <v>44507</v>
       </c>
-      <c r="D59" s="249" t="s">
+      <c r="D59" s="259" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="250"/>
+      <c r="E59" s="260"/>
       <c r="F59" s="121">
         <v>192529.4</v>
       </c>
-      <c r="I59" s="251" t="s">
+      <c r="I59" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="252"/>
-      <c r="K59" s="253">
+      <c r="J59" s="262"/>
+      <c r="K59" s="263">
         <f>K55+K57</f>
         <v>43862.670000000129</v>
       </c>
-      <c r="L59" s="253"/>
+      <c r="L59" s="263"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -18545,23 +18606,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="270"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="280"/>
+      <c r="C1" s="289" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
+      <c r="I1" s="290"/>
+      <c r="J1" s="290"/>
+      <c r="K1" s="290"/>
+      <c r="L1" s="290"/>
+      <c r="M1" s="290"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="271"/>
+      <c r="B2" s="281"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -18571,17 +18632,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="273"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="274" t="s">
+      <c r="H3" s="284" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="274"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -18597,14 +18658,14 @@
       <c r="D4" s="16">
         <v>44507</v>
       </c>
-      <c r="E4" s="275" t="s">
+      <c r="E4" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="276"/>
-      <c r="H4" s="277" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="278"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -18614,10 +18675,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="264" t="s">
+      <c r="P4" s="274" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="265"/>
+      <c r="Q4" s="275"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -20081,11 +20142,11 @@
       <c r="J40" s="67"/>
       <c r="K40" s="82"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="266">
+      <c r="M40" s="276">
         <f>SUM(M5:M39)</f>
         <v>1799884</v>
       </c>
-      <c r="N40" s="268">
+      <c r="N40" s="278">
         <f>SUM(N5:N39)</f>
         <v>38112</v>
       </c>
@@ -20111,8 +20172,8 @@
       <c r="J41" s="67"/>
       <c r="K41" s="71"/>
       <c r="L41" s="69"/>
-      <c r="M41" s="267"/>
-      <c r="N41" s="269"/>
+      <c r="M41" s="277"/>
+      <c r="N41" s="279"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -20327,29 +20388,29 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="254" t="s">
+      <c r="H53" s="264" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="255"/>
+      <c r="I53" s="265"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="256">
+      <c r="K53" s="266">
         <f>I51+L51</f>
         <v>56500.68</v>
       </c>
-      <c r="L53" s="257"/>
-      <c r="M53" s="245">
+      <c r="L53" s="267"/>
+      <c r="M53" s="255">
         <f>N40+M40</f>
         <v>1837996</v>
       </c>
-      <c r="N53" s="246"/>
+      <c r="N53" s="256"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="258" t="s">
+      <c r="D54" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="258"/>
+      <c r="E54" s="268"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
         <v>1829990.32</v>
@@ -20360,22 +20421,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="259" t="s">
+      <c r="D55" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="259"/>
+      <c r="E55" s="269"/>
       <c r="F55" s="102">
         <v>-1751881.55</v>
       </c>
-      <c r="I55" s="260" t="s">
+      <c r="I55" s="270" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="261"/>
-      <c r="K55" s="262">
+      <c r="J55" s="271"/>
+      <c r="K55" s="272">
         <f>F57+F58+F59</f>
         <v>86914.770000000019</v>
       </c>
-      <c r="L55" s="263"/>
+      <c r="L55" s="273"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -20406,11 +20467,11 @@
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="247">
+      <c r="K57" s="257">
         <f>-C4</f>
         <v>-192529.4</v>
       </c>
-      <c r="L57" s="248"/>
+      <c r="L57" s="258"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -20425,22 +20486,22 @@
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="120"/>
-      <c r="D59" s="249" t="s">
+      <c r="D59" s="259" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="250"/>
+      <c r="E59" s="260"/>
       <c r="F59" s="121">
         <v>0</v>
       </c>
-      <c r="I59" s="251" t="s">
+      <c r="I59" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="252"/>
-      <c r="K59" s="253">
+      <c r="J59" s="262"/>
+      <c r="K59" s="263">
         <f>K55+K57</f>
         <v>-105614.62999999998</v>
       </c>
-      <c r="L59" s="253"/>
+      <c r="L59" s="263"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>
@@ -22193,8 +22254,8 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22216,23 +22277,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="270"/>
-      <c r="C1" s="279" t="s">
+      <c r="B1" s="280"/>
+      <c r="C1" s="289" t="s">
         <v>322</v>
       </c>
-      <c r="D1" s="280"/>
-      <c r="E1" s="280"/>
-      <c r="F1" s="280"/>
-      <c r="G1" s="280"/>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
-      <c r="K1" s="280"/>
-      <c r="L1" s="280"/>
-      <c r="M1" s="280"/>
+      <c r="D1" s="290"/>
+      <c r="E1" s="290"/>
+      <c r="F1" s="290"/>
+      <c r="G1" s="290"/>
+      <c r="H1" s="290"/>
+      <c r="I1" s="290"/>
+      <c r="J1" s="290"/>
+      <c r="K1" s="290"/>
+      <c r="L1" s="290"/>
+      <c r="M1" s="290"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="271"/>
+      <c r="B2" s="281"/>
       <c r="C2" s="4"/>
       <c r="H2" s="6"/>
       <c r="I2" s="2"/>
@@ -22242,17 +22303,17 @@
       <c r="N2" s="9"/>
     </row>
     <row r="3" spans="1:18" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="272" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="273"/>
+      <c r="B3" s="282" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="283"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
-      <c r="H3" s="274" t="s">
+      <c r="H3" s="284" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="274"/>
+      <c r="I3" s="284"/>
       <c r="K3" s="136"/>
       <c r="L3" s="136"/>
       <c r="M3" s="137"/>
@@ -22268,14 +22329,14 @@
       <c r="D4" s="16">
         <v>44535</v>
       </c>
-      <c r="E4" s="275" t="s">
+      <c r="E4" s="285" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="276"/>
-      <c r="H4" s="277" t="s">
+      <c r="F4" s="286"/>
+      <c r="H4" s="287" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="278"/>
+      <c r="I4" s="288"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
       <c r="L4" s="19"/>
@@ -22285,10 +22346,10 @@
       <c r="N4" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="P4" s="264" t="s">
+      <c r="P4" s="274" t="s">
         <v>28</v>
       </c>
-      <c r="Q4" s="265"/>
+      <c r="Q4" s="275"/>
     </row>
     <row r="5" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
@@ -22538,7 +22599,7 @@
         <v>44541</v>
       </c>
       <c r="K10" s="42" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="L10" s="43">
         <v>11000</v>
@@ -22613,7 +22674,7 @@
         <v>1062</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E12" s="24">
         <v>44543</v>
@@ -22763,18 +22824,19 @@
       <c r="K15" s="40"/>
       <c r="L15" s="35"/>
       <c r="M15" s="138">
-        <v>0</v>
+        <f>40000+24340+25000</f>
+        <v>89340</v>
       </c>
       <c r="N15" s="30">
-        <v>0</v>
+        <v>16270</v>
       </c>
       <c r="P15" s="83">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>105653</v>
       </c>
       <c r="Q15" s="136">
         <f t="shared" si="1"/>
-        <v>-105605</v>
+        <v>5</v>
       </c>
       <c r="R15" s="26"/>
     </row>
@@ -22784,34 +22846,41 @@
         <v>44547</v>
       </c>
       <c r="C16" s="22">
-        <v>0</v>
-      </c>
-      <c r="D16" s="31"/>
+        <v>3120</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>267</v>
+      </c>
       <c r="E16" s="24">
         <v>44547</v>
       </c>
-      <c r="F16" s="25"/>
+      <c r="F16" s="25">
+        <v>86325</v>
+      </c>
       <c r="G16" s="26"/>
       <c r="H16" s="32">
         <v>44547</v>
       </c>
-      <c r="I16" s="28"/>
+      <c r="I16" s="28">
+        <v>51</v>
+      </c>
       <c r="J16" s="33"/>
       <c r="K16" s="40"/>
       <c r="L16" s="9"/>
       <c r="M16" s="138">
-        <v>0</v>
+        <f>30000+30000+20690</f>
+        <v>80690</v>
       </c>
       <c r="N16" s="30">
-        <v>0</v>
+        <v>2460</v>
       </c>
       <c r="P16" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q16" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>86321</v>
+      </c>
+      <c r="Q16" s="211">
+        <f t="shared" si="1"/>
+        <v>-4</v>
       </c>
       <c r="R16" s="26"/>
     </row>
@@ -22827,28 +22896,40 @@
       <c r="E17" s="24">
         <v>44548</v>
       </c>
-      <c r="F17" s="25"/>
+      <c r="F17" s="25">
+        <v>103705</v>
+      </c>
       <c r="G17" s="26"/>
       <c r="H17" s="32">
         <v>44548</v>
       </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="43"/>
+      <c r="I17" s="28">
+        <v>36</v>
+      </c>
+      <c r="J17" s="33">
+        <v>44548</v>
+      </c>
+      <c r="K17" s="245" t="s">
+        <v>327</v>
+      </c>
+      <c r="L17" s="43">
+        <f>12786+17357</f>
+        <v>30143</v>
+      </c>
       <c r="M17" s="138">
-        <v>0</v>
+        <f>15920+50000</f>
+        <v>65920</v>
       </c>
       <c r="N17" s="30">
-        <v>0</v>
+        <v>7608</v>
       </c>
       <c r="P17" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>103707</v>
       </c>
       <c r="Q17" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R17" s="26"/>
     </row>
@@ -22864,28 +22945,33 @@
       <c r="E18" s="24">
         <v>44549</v>
       </c>
-      <c r="F18" s="25"/>
+      <c r="F18" s="25">
+        <v>110543</v>
+      </c>
       <c r="G18" s="26"/>
       <c r="H18" s="32">
         <v>44549</v>
       </c>
-      <c r="I18" s="28"/>
+      <c r="I18" s="28">
+        <v>15</v>
+      </c>
       <c r="J18" s="33"/>
       <c r="K18" s="47"/>
       <c r="L18" s="35"/>
       <c r="M18" s="138">
-        <v>0</v>
+        <f>90000+19450</f>
+        <v>109450</v>
       </c>
       <c r="N18" s="30">
-        <v>0</v>
+        <v>1082</v>
       </c>
       <c r="P18" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>110547</v>
       </c>
       <c r="Q18" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R18" s="26"/>
     </row>
@@ -22901,28 +22987,33 @@
       <c r="E19" s="24">
         <v>44550</v>
       </c>
-      <c r="F19" s="25"/>
+      <c r="F19" s="25">
+        <v>71144</v>
+      </c>
       <c r="G19" s="26"/>
       <c r="H19" s="32">
         <v>44550</v>
       </c>
-      <c r="I19" s="28"/>
+      <c r="I19" s="28">
+        <v>52</v>
+      </c>
       <c r="J19" s="33"/>
       <c r="K19" s="48"/>
       <c r="L19" s="49"/>
       <c r="M19" s="138">
-        <v>0</v>
+        <f>35000+35970</f>
+        <v>70970</v>
       </c>
       <c r="N19" s="30">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="P19" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>71142</v>
+      </c>
+      <c r="Q19" s="211">
+        <f t="shared" si="1"/>
+        <v>-2</v>
       </c>
       <c r="R19" s="26"/>
     </row>
@@ -22932,34 +23023,41 @@
         <v>44551</v>
       </c>
       <c r="C20" s="22">
-        <v>0</v>
-      </c>
-      <c r="D20" s="31"/>
+        <v>3400</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>267</v>
+      </c>
       <c r="E20" s="24">
         <v>44551</v>
       </c>
-      <c r="F20" s="25"/>
+      <c r="F20" s="25">
+        <v>99474</v>
+      </c>
       <c r="G20" s="26"/>
       <c r="H20" s="32">
         <v>44551</v>
       </c>
-      <c r="I20" s="28"/>
+      <c r="I20" s="28">
+        <v>154</v>
+      </c>
       <c r="J20" s="33"/>
       <c r="K20" s="50"/>
       <c r="L20" s="43"/>
       <c r="M20" s="138">
-        <v>0</v>
+        <f>50000+43150</f>
+        <v>93150</v>
       </c>
       <c r="N20" s="30">
-        <v>0</v>
+        <v>2787</v>
       </c>
       <c r="P20" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>99491</v>
       </c>
       <c r="Q20" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="R20" s="26"/>
     </row>
@@ -22969,34 +23067,42 @@
         <v>44552</v>
       </c>
       <c r="C21" s="22">
-        <v>0</v>
-      </c>
-      <c r="D21" s="31"/>
+        <f>33259+28</f>
+        <v>33287</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>325</v>
+      </c>
       <c r="E21" s="24">
         <v>44552</v>
       </c>
-      <c r="F21" s="25"/>
+      <c r="F21" s="25">
+        <v>126486</v>
+      </c>
       <c r="G21" s="26"/>
       <c r="H21" s="32">
         <v>44552</v>
       </c>
-      <c r="I21" s="28"/>
+      <c r="I21" s="28">
+        <v>152</v>
+      </c>
       <c r="J21" s="33"/>
       <c r="K21" s="177"/>
       <c r="L21" s="43"/>
       <c r="M21" s="138">
-        <v>0</v>
+        <f>35000+40000+17550</f>
+        <v>92550</v>
       </c>
       <c r="N21" s="30">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="P21" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>126489</v>
       </c>
       <c r="Q21" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R21" s="26"/>
     </row>
@@ -23012,28 +23118,33 @@
       <c r="E22" s="24">
         <v>44553</v>
       </c>
-      <c r="F22" s="25"/>
+      <c r="F22" s="25">
+        <v>154210</v>
+      </c>
       <c r="G22" s="26"/>
       <c r="H22" s="32">
         <v>44553</v>
       </c>
-      <c r="I22" s="28"/>
+      <c r="I22" s="28">
+        <v>133</v>
+      </c>
       <c r="J22" s="33"/>
       <c r="K22" s="51"/>
       <c r="L22" s="52"/>
       <c r="M22" s="138">
-        <v>0</v>
+        <f>60000+65000+27050</f>
+        <v>152050</v>
       </c>
       <c r="N22" s="30">
-        <v>0</v>
+        <v>2030</v>
       </c>
       <c r="P22" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>154213</v>
       </c>
       <c r="Q22" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R22" s="26"/>
     </row>
@@ -23049,28 +23160,39 @@
       <c r="E23" s="24">
         <v>44554</v>
       </c>
-      <c r="F23" s="25"/>
+      <c r="F23" s="25">
+        <v>157979</v>
+      </c>
       <c r="G23" s="26"/>
       <c r="H23" s="32">
         <v>44554</v>
       </c>
-      <c r="I23" s="28"/>
-      <c r="J23" s="53"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="43"/>
+      <c r="I23" s="28">
+        <v>322</v>
+      </c>
+      <c r="J23" s="53">
+        <v>44554</v>
+      </c>
+      <c r="K23" s="54" t="s">
+        <v>326</v>
+      </c>
+      <c r="L23" s="43">
+        <v>14586</v>
+      </c>
       <c r="M23" s="138">
-        <v>0</v>
+        <f>80000+30000+22570</f>
+        <v>132570</v>
       </c>
       <c r="N23" s="30">
-        <v>0</v>
+        <v>10498</v>
       </c>
       <c r="P23" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q23" s="136">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>157976</v>
+      </c>
+      <c r="Q23" s="217">
+        <f t="shared" si="1"/>
+        <v>-3</v>
       </c>
       <c r="R23" s="26"/>
     </row>
@@ -23079,26 +23201,34 @@
       <c r="B24" s="21">
         <v>44555</v>
       </c>
-      <c r="C24" s="22">
-        <v>0</v>
-      </c>
-      <c r="D24" s="31"/>
+      <c r="C24" s="246">
+        <v>0</v>
+      </c>
+      <c r="D24" s="253" t="s">
+        <v>329</v>
+      </c>
       <c r="E24" s="24">
         <v>44555</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="32">
+      <c r="F24" s="247"/>
+      <c r="G24" s="248"/>
+      <c r="H24" s="249">
         <v>44555</v>
       </c>
-      <c r="I24" s="28"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="138">
-        <v>0</v>
-      </c>
-      <c r="N24" s="30">
+      <c r="I24" s="250"/>
+      <c r="J24" s="254" t="s">
+        <v>329</v>
+      </c>
+      <c r="K24" s="56">
+        <v>0</v>
+      </c>
+      <c r="L24" s="57">
+        <v>0</v>
+      </c>
+      <c r="M24" s="251">
+        <v>0</v>
+      </c>
+      <c r="N24" s="252">
         <v>0</v>
       </c>
       <c r="P24" s="83">
@@ -23123,31 +23253,36 @@
       <c r="E25" s="24">
         <v>44556</v>
       </c>
-      <c r="F25" s="25"/>
+      <c r="F25" s="25">
+        <v>123482</v>
+      </c>
       <c r="G25" s="26"/>
       <c r="H25" s="32">
         <v>44556</v>
       </c>
-      <c r="I25" s="28"/>
+      <c r="I25" s="28">
+        <v>15</v>
+      </c>
       <c r="J25" s="58"/>
       <c r="K25" s="59"/>
       <c r="L25" s="60"/>
       <c r="M25" s="138">
-        <v>0</v>
+        <f>100000+22425</f>
+        <v>122425</v>
       </c>
       <c r="N25" s="30">
-        <v>0</v>
+        <v>1043</v>
       </c>
       <c r="O25" t="s">
         <v>4</v>
       </c>
       <c r="P25" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>123483</v>
       </c>
       <c r="Q25" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R25" s="26"/>
       <c r="S25" t="s">
@@ -23160,34 +23295,41 @@
         <v>44557</v>
       </c>
       <c r="C26" s="22">
-        <v>0</v>
-      </c>
-      <c r="D26" s="31"/>
+        <v>4234</v>
+      </c>
+      <c r="D26" s="31" t="s">
+        <v>267</v>
+      </c>
       <c r="E26" s="24">
         <v>44557</v>
       </c>
-      <c r="F26" s="25"/>
+      <c r="F26" s="25">
+        <v>65323</v>
+      </c>
       <c r="G26" s="26"/>
       <c r="H26" s="32">
         <v>44557</v>
       </c>
-      <c r="I26" s="28"/>
+      <c r="I26" s="28">
+        <v>15</v>
+      </c>
       <c r="J26" s="33"/>
       <c r="K26" s="56"/>
       <c r="L26" s="43"/>
       <c r="M26" s="138">
-        <v>0</v>
+        <f>25000+35875</f>
+        <v>60875</v>
       </c>
       <c r="N26" s="30">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P26" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>65324</v>
       </c>
       <c r="Q26" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="51"/>
     </row>
@@ -23197,34 +23339,47 @@
         <v>44558</v>
       </c>
       <c r="C27" s="22">
-        <v>0</v>
-      </c>
-      <c r="D27" s="38"/>
+        <v>5253</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>330</v>
+      </c>
       <c r="E27" s="24">
         <v>44558</v>
       </c>
-      <c r="F27" s="25"/>
+      <c r="F27" s="25">
+        <v>66810</v>
+      </c>
       <c r="G27" s="26"/>
       <c r="H27" s="32">
         <v>44558</v>
       </c>
-      <c r="I27" s="28"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="60"/>
+      <c r="I27" s="28">
+        <v>44</v>
+      </c>
+      <c r="J27" s="65">
+        <v>44558</v>
+      </c>
+      <c r="K27" s="62" t="s">
+        <v>331</v>
+      </c>
+      <c r="L27" s="60">
+        <v>16500</v>
+      </c>
       <c r="M27" s="138">
-        <v>0</v>
+        <f>30000+15055</f>
+        <v>45055</v>
       </c>
       <c r="N27" s="30">
         <v>0</v>
       </c>
       <c r="P27" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>66852</v>
       </c>
       <c r="Q27" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="R27" s="26"/>
     </row>
@@ -23234,34 +23389,41 @@
         <v>44559</v>
       </c>
       <c r="C28" s="22">
-        <v>0</v>
-      </c>
-      <c r="D28" s="38"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>275</v>
+      </c>
       <c r="E28" s="24">
         <v>44559</v>
       </c>
-      <c r="F28" s="25"/>
+      <c r="F28" s="25">
+        <v>92430</v>
+      </c>
       <c r="G28" s="26"/>
       <c r="H28" s="32">
         <v>44559</v>
       </c>
-      <c r="I28" s="28"/>
+      <c r="I28" s="28">
+        <v>36</v>
+      </c>
       <c r="J28" s="63"/>
       <c r="K28" s="34"/>
       <c r="L28" s="60"/>
       <c r="M28" s="138">
-        <v>0</v>
+        <f>45000+47210</f>
+        <v>92210</v>
       </c>
       <c r="N28" s="30">
-        <v>0</v>
+        <v>161</v>
       </c>
       <c r="P28" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>92431</v>
       </c>
       <c r="Q28" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R28" s="26"/>
     </row>
@@ -23277,28 +23439,33 @@
       <c r="E29" s="24">
         <v>44560</v>
       </c>
-      <c r="F29" s="25"/>
+      <c r="F29" s="25">
+        <v>115083</v>
+      </c>
       <c r="G29" s="26"/>
       <c r="H29" s="32">
         <v>44560</v>
       </c>
-      <c r="I29" s="28"/>
+      <c r="I29" s="28">
+        <v>0</v>
+      </c>
       <c r="J29" s="65"/>
       <c r="K29" s="66"/>
       <c r="L29" s="60"/>
       <c r="M29" s="138">
-        <v>0</v>
+        <f>40000+28410+45000</f>
+        <v>113410</v>
       </c>
       <c r="N29" s="30">
-        <v>0</v>
+        <v>1671</v>
       </c>
       <c r="P29" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>115081</v>
       </c>
       <c r="Q29" s="136">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="R29" s="26"/>
     </row>
@@ -23314,28 +23481,39 @@
       <c r="E30" s="24">
         <v>44561</v>
       </c>
-      <c r="F30" s="25"/>
+      <c r="F30" s="25">
+        <v>147231</v>
+      </c>
       <c r="G30" s="26"/>
       <c r="H30" s="32">
         <v>44561</v>
       </c>
-      <c r="I30" s="28"/>
-      <c r="J30" s="67"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="138">
-        <v>0</v>
+      <c r="I30" s="28">
+        <v>36</v>
+      </c>
+      <c r="J30" s="67">
+        <v>44561</v>
+      </c>
+      <c r="K30" s="68" t="s">
+        <v>332</v>
+      </c>
+      <c r="L30" s="69">
+        <v>12129</v>
+      </c>
+      <c r="M30" s="297">
+        <f>100000</f>
+        <v>100000</v>
       </c>
       <c r="N30" s="30">
-        <v>0</v>
+        <v>9300</v>
       </c>
       <c r="P30" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q30" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>121465</v>
+      </c>
+      <c r="Q30" s="298">
+        <f t="shared" si="1"/>
+        <v>-25766</v>
       </c>
       <c r="R30" s="26"/>
     </row>
@@ -23344,26 +23522,34 @@
       <c r="B31" s="21">
         <v>44562</v>
       </c>
-      <c r="C31" s="22">
-        <v>0</v>
-      </c>
-      <c r="D31" s="70"/>
+      <c r="C31" s="299">
+        <v>0</v>
+      </c>
+      <c r="D31" s="300" t="s">
+        <v>329</v>
+      </c>
       <c r="E31" s="24">
         <v>44562</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="32">
+      <c r="F31" s="301">
+        <v>0</v>
+      </c>
+      <c r="G31" s="302"/>
+      <c r="H31" s="303">
         <v>44562</v>
       </c>
-      <c r="I31" s="28"/>
-      <c r="J31" s="67"/>
+      <c r="I31" s="304">
+        <v>0</v>
+      </c>
+      <c r="J31" s="305" t="s">
+        <v>329</v>
+      </c>
       <c r="K31" s="71"/>
       <c r="L31" s="72"/>
-      <c r="M31" s="138">
-        <v>0</v>
-      </c>
-      <c r="N31" s="30">
+      <c r="M31" s="306">
+        <v>0</v>
+      </c>
+      <c r="N31" s="307">
         <v>0</v>
       </c>
       <c r="P31" s="83">
@@ -23382,34 +23568,41 @@
         <v>44563</v>
       </c>
       <c r="C32" s="22">
-        <v>0</v>
-      </c>
-      <c r="D32" s="73"/>
+        <v>31365</v>
+      </c>
+      <c r="D32" s="73" t="s">
+        <v>333</v>
+      </c>
       <c r="E32" s="24">
         <v>44563</v>
       </c>
-      <c r="F32" s="25"/>
+      <c r="F32" s="25">
+        <v>82275</v>
+      </c>
       <c r="G32" s="26"/>
       <c r="H32" s="32">
         <v>44563</v>
       </c>
-      <c r="I32" s="28"/>
+      <c r="I32" s="28">
+        <v>43</v>
+      </c>
       <c r="J32" s="67"/>
       <c r="K32" s="68"/>
       <c r="L32" s="69"/>
-      <c r="M32" s="138">
-        <v>0</v>
+      <c r="M32" s="297">
+        <f>16727</f>
+        <v>16727</v>
       </c>
       <c r="N32" s="30">
-        <v>0</v>
+        <v>640</v>
       </c>
       <c r="P32" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q32" s="9">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <v>48775</v>
+      </c>
+      <c r="Q32" s="298">
+        <f t="shared" si="1"/>
+        <v>-33500</v>
       </c>
       <c r="R32" s="26"/>
     </row>
@@ -23626,21 +23819,21 @@
       <c r="J40" s="67"/>
       <c r="K40" s="82"/>
       <c r="L40" s="69"/>
-      <c r="M40" s="266">
+      <c r="M40" s="276">
         <f>SUM(M5:M39)</f>
-        <v>663162</v>
-      </c>
-      <c r="N40" s="268">
+        <v>2100554</v>
+      </c>
+      <c r="N40" s="278">
         <f>SUM(N5:N39)</f>
-        <v>14207</v>
+        <v>70577</v>
       </c>
       <c r="P40" s="83">
         <f>SUM(P5:P39)</f>
-        <v>715108</v>
+        <v>2364015</v>
       </c>
       <c r="Q40" s="222">
         <f>SUM(Q5:Q38)</f>
-        <v>-96802</v>
+        <v>-50395</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -23656,8 +23849,8 @@
       <c r="J41" s="67"/>
       <c r="K41" s="71"/>
       <c r="L41" s="69"/>
-      <c r="M41" s="267"/>
-      <c r="N41" s="269"/>
+      <c r="M41" s="277"/>
+      <c r="N41" s="279"/>
       <c r="P41" s="83"/>
       <c r="Q41" s="9"/>
     </row>
@@ -23830,7 +24023,7 @@
       </c>
       <c r="C51" s="93">
         <f>SUM(C5:C50)</f>
-        <v>24906</v>
+        <v>105589</v>
       </c>
       <c r="D51" s="94"/>
       <c r="E51" s="95" t="s">
@@ -23838,7 +24031,7 @@
       </c>
       <c r="F51" s="96">
         <f>SUM(F5:F50)</f>
-        <v>811910</v>
+        <v>2414410</v>
       </c>
       <c r="G51" s="94"/>
       <c r="H51" s="97" t="s">
@@ -23846,7 +24039,7 @@
       </c>
       <c r="I51" s="98">
         <f>SUM(I5:I50)</f>
-        <v>1833</v>
+        <v>2937</v>
       </c>
       <c r="J51" s="99"/>
       <c r="K51" s="100" t="s">
@@ -23854,7 +24047,7 @@
       </c>
       <c r="L51" s="101">
         <f>SUM(L5:L50)</f>
-        <v>11000</v>
+        <v>84358</v>
       </c>
       <c r="M51" s="102"/>
       <c r="N51" s="102"/>
@@ -23872,32 +24065,32 @@
       <c r="A53" s="104"/>
       <c r="B53" s="105"/>
       <c r="C53" s="3"/>
-      <c r="H53" s="254" t="s">
+      <c r="H53" s="264" t="s">
         <v>8</v>
       </c>
-      <c r="I53" s="255"/>
+      <c r="I53" s="265"/>
       <c r="J53" s="106"/>
-      <c r="K53" s="256">
+      <c r="K53" s="266">
         <f>I51+L51</f>
-        <v>12833</v>
-      </c>
-      <c r="L53" s="257"/>
-      <c r="M53" s="245">
+        <v>87295</v>
+      </c>
+      <c r="L53" s="267"/>
+      <c r="M53" s="255">
         <f>N40+M40</f>
-        <v>677369</v>
-      </c>
-      <c r="N53" s="246"/>
+        <v>2171131</v>
+      </c>
+      <c r="N53" s="256"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="9"/>
     </row>
     <row r="54" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D54" s="258" t="s">
+      <c r="D54" s="268" t="s">
         <v>9</v>
       </c>
-      <c r="E54" s="258"/>
+      <c r="E54" s="268"/>
       <c r="F54" s="107">
         <f>F51-K53-C51</f>
-        <v>774171</v>
+        <v>2221526</v>
       </c>
       <c r="I54" s="108"/>
       <c r="J54" s="109"/>
@@ -23905,22 +24098,22 @@
       <c r="Q54" s="9"/>
     </row>
     <row r="55" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="D55" s="259" t="s">
+      <c r="D55" s="269" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="259"/>
+      <c r="E55" s="269"/>
       <c r="F55" s="102">
         <v>0</v>
       </c>
-      <c r="I55" s="260" t="s">
+      <c r="I55" s="270" t="s">
         <v>11</v>
       </c>
-      <c r="J55" s="261"/>
-      <c r="K55" s="262">
+      <c r="J55" s="271"/>
+      <c r="K55" s="272">
         <f>F57+F58+F59</f>
-        <v>774171</v>
-      </c>
-      <c r="L55" s="263"/>
+        <v>2221526</v>
+      </c>
+      <c r="L55" s="273"/>
       <c r="P55" s="83"/>
       <c r="Q55" s="9"/>
     </row>
@@ -23944,18 +24137,18 @@
       </c>
       <c r="F57" s="102">
         <f>SUM(F54:F56)</f>
-        <v>774171</v>
+        <v>2221526</v>
       </c>
       <c r="H57" s="20"/>
       <c r="I57" s="116" t="s">
         <v>13</v>
       </c>
       <c r="J57" s="117"/>
-      <c r="K57" s="247">
+      <c r="K57" s="257">
         <f>-C4</f>
         <v>0</v>
       </c>
-      <c r="L57" s="248"/>
+      <c r="L57" s="258"/>
     </row>
     <row r="58" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="118" t="s">
@@ -23970,22 +24163,22 @@
     </row>
     <row r="59" spans="1:17" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="120"/>
-      <c r="D59" s="249" t="s">
+      <c r="D59" s="259" t="s">
         <v>16</v>
       </c>
-      <c r="E59" s="250"/>
+      <c r="E59" s="260"/>
       <c r="F59" s="121">
         <v>0</v>
       </c>
-      <c r="I59" s="251" t="s">
+      <c r="I59" s="261" t="s">
         <v>17</v>
       </c>
-      <c r="J59" s="252"/>
-      <c r="K59" s="253">
+      <c r="J59" s="262"/>
+      <c r="K59" s="263">
         <f>K55+K57</f>
-        <v>774171</v>
-      </c>
-      <c r="L59" s="253"/>
+        <v>2221526</v>
+      </c>
+      <c r="L59" s="263"/>
     </row>
     <row r="60" spans="1:17" ht="17.25" x14ac:dyDescent="0.3">
       <c r="C60" s="122"/>

</xml_diff>